<commit_message>
finalized data cleaning and uploading
</commit_message>
<xml_diff>
--- a/data/consumption_data.xlsx
+++ b/data/consumption_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779C0031-75DD-9643-B220-D244F8C0B485}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A333AB2-5D58-C24C-B0CB-C4D2DB246DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="35820" windowHeight="20420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14560" yWindow="2460" windowWidth="21500" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10543" uniqueCount="1361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10542" uniqueCount="1361">
   <si>
     <t>Sun &amp; Chen-2014-Aquaculture</t>
   </si>
@@ -4536,8 +4536,8 @@
   <dimension ref="A1:Y627"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A591" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D623" sqref="D623"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8029,11 +8029,11 @@
       <c r="B54" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="4">
+        <v>22</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>1360</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>1352</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Updated all data sets, can proceed to re-analzing data now
</commit_message>
<xml_diff>
--- a/data/consumption_data.xlsx
+++ b/data/consumption_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B543FFE-E052-204C-92CE-35587AAF0324}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DE687A-EAFB-EB41-B8E3-656659B84150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15220" yWindow="460" windowWidth="28520" windowHeight="19300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="1380" windowWidth="28520" windowHeight="19300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -1059,9 +1059,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y639"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A603" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T618" sqref="T618"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A393" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T400" sqref="T400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1076,8 +1076,8 @@
     <col min="9" max="9" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.5" style="4" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
updated e-mail list and reference in consumption data
</commit_message>
<xml_diff>
--- a/data/consumption_data.xlsx
+++ b/data/consumption_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153F8470-E90F-1B42-808B-239B7E74A75D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E57B6AF-FB33-A34F-83E8-F26F030189F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7660" yWindow="500" windowWidth="28520" windowHeight="19300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="780" windowWidth="28520" windowHeight="19300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -531,9 +531,6 @@
     <t>Hayward&amp;Arnold-1996-Trans.Am.Fish.Soc</t>
   </si>
   <si>
-    <t>Chipps&amp;Whal-1996-Trans.Am.Fish.Soc</t>
-  </si>
-  <si>
     <t>Wang-etal-2003-JournaloftheWorldAquacultureSociety</t>
   </si>
   <si>
@@ -592,6 +589,9 @@
   </si>
   <si>
     <t>Wootton-etal-1980-J.Fish.Bio</t>
+  </si>
+  <si>
+    <t>Chipps&amp;Whal-2004-Trans.Am.Fish.Soc</t>
   </si>
 </sst>
 </file>
@@ -1064,8 +1064,8 @@
   <dimension ref="A1:Y639"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A611" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X632" sqref="X632"/>
+      <pane ySplit="1" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W219" sqref="W219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2547,10 +2547,10 @@
         <v>5.7</v>
       </c>
       <c r="U22" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V22" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
@@ -2615,10 +2615,10 @@
         <v>5.7</v>
       </c>
       <c r="U23" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V23" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
@@ -2683,10 +2683,10 @@
         <v>5.7</v>
       </c>
       <c r="U24" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V24" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V24" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
@@ -2751,10 +2751,10 @@
         <v>5.7</v>
       </c>
       <c r="U25" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V25" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V25" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
@@ -2819,10 +2819,10 @@
         <v>5.7</v>
       </c>
       <c r="U26" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V26" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V26" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.2">
@@ -2887,10 +2887,10 @@
         <v>5.7</v>
       </c>
       <c r="U27" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V27" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V27" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
@@ -2955,10 +2955,10 @@
         <v>5.7</v>
       </c>
       <c r="U28" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V28" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V28" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
@@ -3023,10 +3023,10 @@
         <v>5.7</v>
       </c>
       <c r="U29" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V29" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V29" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3091,10 +3091,10 @@
         <v>5.7</v>
       </c>
       <c r="U30" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V30" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V30" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="W30" s="4"/>
       <c r="X30" s="4"/>
@@ -3162,10 +3162,10 @@
         <v>5.7</v>
       </c>
       <c r="U31" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V31" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V31" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
@@ -3230,10 +3230,10 @@
         <v>5.7</v>
       </c>
       <c r="U32" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V32" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V32" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.2">
@@ -3298,10 +3298,10 @@
         <v>5.7</v>
       </c>
       <c r="U33" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V33" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V33" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.2">
@@ -3366,10 +3366,10 @@
         <v>5.7</v>
       </c>
       <c r="U34" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V34" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V34" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.2">
@@ -3434,10 +3434,10 @@
         <v>5.7</v>
       </c>
       <c r="U35" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V35" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V35" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.2">
@@ -3502,10 +3502,10 @@
         <v>5.7</v>
       </c>
       <c r="U36" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V36" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V36" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.2">
@@ -3570,10 +3570,10 @@
         <v>5.7</v>
       </c>
       <c r="U37" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V37" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V37" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.2">
@@ -3638,10 +3638,10 @@
         <v>5.7</v>
       </c>
       <c r="U38" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V38" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V38" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.2">
@@ -3706,10 +3706,10 @@
         <v>5.7</v>
       </c>
       <c r="U39" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V39" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V39" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
@@ -3774,10 +3774,10 @@
         <v>5.7</v>
       </c>
       <c r="U40" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V40" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V40" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.2">
@@ -3842,10 +3842,10 @@
         <v>5.7</v>
       </c>
       <c r="U41" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V41" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V41" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
@@ -3910,10 +3910,10 @@
         <v>5.7</v>
       </c>
       <c r="U42" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V42" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V42" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.2">
@@ -3978,10 +3978,10 @@
         <v>5.7</v>
       </c>
       <c r="U43" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V43" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V43" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.2">
@@ -4046,10 +4046,10 @@
         <v>5.7</v>
       </c>
       <c r="U44" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V44" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V44" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.2">
@@ -4114,10 +4114,10 @@
         <v>5.7</v>
       </c>
       <c r="U45" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V45" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V45" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.2">
@@ -4182,10 +4182,10 @@
         <v>5.7</v>
       </c>
       <c r="U46" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V46" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V46" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.2">
@@ -4250,10 +4250,10 @@
         <v>5.7</v>
       </c>
       <c r="U47" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V47" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V47" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.2">
@@ -4318,10 +4318,10 @@
         <v>5.7</v>
       </c>
       <c r="U48" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V48" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V48" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
@@ -4386,10 +4386,10 @@
         <v>5.7</v>
       </c>
       <c r="U49" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V49" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V49" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
@@ -4454,10 +4454,10 @@
         <v>5.7</v>
       </c>
       <c r="U50" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V50" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V50" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.2">
@@ -4522,10 +4522,10 @@
         <v>5.7</v>
       </c>
       <c r="U51" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V51" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V51" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
@@ -4590,10 +4590,10 @@
         <v>5.7</v>
       </c>
       <c r="U52" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V52" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V52" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.2">
@@ -4658,10 +4658,10 @@
         <v>5.7</v>
       </c>
       <c r="U53" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V53" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V53" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.2">
@@ -4726,10 +4726,10 @@
         <v>5.7</v>
       </c>
       <c r="U54" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V54" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V54" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
@@ -4794,10 +4794,10 @@
         <v>5.7</v>
       </c>
       <c r="U55" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V55" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V55" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
@@ -4862,10 +4862,10 @@
         <v>5.7</v>
       </c>
       <c r="U56" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V56" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V56" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.2">
@@ -4930,10 +4930,10 @@
         <v>5.7</v>
       </c>
       <c r="U57" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V57" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V57" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
@@ -4998,10 +4998,10 @@
         <v>5.7</v>
       </c>
       <c r="U58" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V58" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V58" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
@@ -5066,10 +5066,10 @@
         <v>5.7</v>
       </c>
       <c r="U59" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V59" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V59" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
@@ -5134,10 +5134,10 @@
         <v>5.7</v>
       </c>
       <c r="U60" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V60" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V60" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.2">
@@ -5202,10 +5202,10 @@
         <v>5.7</v>
       </c>
       <c r="U61" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V61" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V61" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
@@ -5270,10 +5270,10 @@
         <v>5.7</v>
       </c>
       <c r="U62" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V62" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V62" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.2">
@@ -5338,10 +5338,10 @@
         <v>5.7</v>
       </c>
       <c r="U63" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V63" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V63" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.2">
@@ -5406,10 +5406,10 @@
         <v>5.7</v>
       </c>
       <c r="U64" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V64" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V64" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.2">
@@ -5474,10 +5474,10 @@
         <v>5.7</v>
       </c>
       <c r="U65" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V65" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V65" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.2">
@@ -5542,10 +5542,10 @@
         <v>5.7</v>
       </c>
       <c r="U66" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V66" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V66" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.2">
@@ -5610,10 +5610,10 @@
         <v>5.7</v>
       </c>
       <c r="U67" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V67" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V67" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.2">
@@ -5678,10 +5678,10 @@
         <v>5.7</v>
       </c>
       <c r="U68" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V68" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V68" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.2">
@@ -5746,10 +5746,10 @@
         <v>5.7</v>
       </c>
       <c r="U69" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V69" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V69" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.2">
@@ -5814,10 +5814,10 @@
         <v>5.7</v>
       </c>
       <c r="U70" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V70" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V70" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.2">
@@ -5882,10 +5882,10 @@
         <v>5.7</v>
       </c>
       <c r="U71" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V71" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V71" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.2">
@@ -5950,10 +5950,10 @@
         <v>5.7</v>
       </c>
       <c r="U72" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V72" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V72" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.2">
@@ -6018,10 +6018,10 @@
         <v>5.7</v>
       </c>
       <c r="U73" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V73" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V73" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.2">
@@ -6086,10 +6086,10 @@
         <v>5.7</v>
       </c>
       <c r="U74" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V74" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V74" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.2">
@@ -6154,10 +6154,10 @@
         <v>5.7</v>
       </c>
       <c r="U75" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V75" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V75" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.2">
@@ -6222,10 +6222,10 @@
         <v>5.7</v>
       </c>
       <c r="U76" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V76" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V76" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.2">
@@ -6290,10 +6290,10 @@
         <v>5.7</v>
       </c>
       <c r="U77" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="V77" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="V77" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.2">
@@ -13433,7 +13433,7 @@
         <v>128</v>
       </c>
       <c r="V182" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="183" spans="1:22" x14ac:dyDescent="0.2">
@@ -13501,7 +13501,7 @@
         <v>128</v>
       </c>
       <c r="V183" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="184" spans="1:22" x14ac:dyDescent="0.2">
@@ -13569,7 +13569,7 @@
         <v>128</v>
       </c>
       <c r="V184" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="185" spans="1:22" x14ac:dyDescent="0.2">
@@ -13637,7 +13637,7 @@
         <v>128</v>
       </c>
       <c r="V185" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="186" spans="1:22" x14ac:dyDescent="0.2">
@@ -13705,7 +13705,7 @@
         <v>128</v>
       </c>
       <c r="V186" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="187" spans="1:22" x14ac:dyDescent="0.2">
@@ -13773,7 +13773,7 @@
         <v>128</v>
       </c>
       <c r="V187" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="188" spans="1:22" x14ac:dyDescent="0.2">
@@ -13841,7 +13841,7 @@
         <v>128</v>
       </c>
       <c r="V188" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="189" spans="1:22" x14ac:dyDescent="0.2">
@@ -13909,7 +13909,7 @@
         <v>128</v>
       </c>
       <c r="V189" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="190" spans="1:22" x14ac:dyDescent="0.2">
@@ -13977,7 +13977,7 @@
         <v>128</v>
       </c>
       <c r="V190" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="191" spans="1:22" x14ac:dyDescent="0.2">
@@ -14045,7 +14045,7 @@
         <v>128</v>
       </c>
       <c r="V191" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="192" spans="1:22" x14ac:dyDescent="0.2">
@@ -14113,7 +14113,7 @@
         <v>128</v>
       </c>
       <c r="V192" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="193" spans="1:22" x14ac:dyDescent="0.2">
@@ -14181,7 +14181,7 @@
         <v>128</v>
       </c>
       <c r="V193" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="194" spans="1:22" x14ac:dyDescent="0.2">
@@ -14249,7 +14249,7 @@
         <v>128</v>
       </c>
       <c r="V194" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="195" spans="1:22" x14ac:dyDescent="0.2">
@@ -14317,7 +14317,7 @@
         <v>128</v>
       </c>
       <c r="V195" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="196" spans="1:22" x14ac:dyDescent="0.2">
@@ -14385,7 +14385,7 @@
         <v>128</v>
       </c>
       <c r="V196" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="197" spans="1:22" x14ac:dyDescent="0.2">
@@ -14453,7 +14453,7 @@
         <v>128</v>
       </c>
       <c r="V197" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="198" spans="1:22" x14ac:dyDescent="0.2">
@@ -14521,7 +14521,7 @@
         <v>128</v>
       </c>
       <c r="V198" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="199" spans="1:22" x14ac:dyDescent="0.2">
@@ -14589,7 +14589,7 @@
         <v>128</v>
       </c>
       <c r="V199" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="200" spans="1:22" x14ac:dyDescent="0.2">
@@ -14657,7 +14657,7 @@
         <v>128</v>
       </c>
       <c r="V200" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="201" spans="1:22" x14ac:dyDescent="0.2">
@@ -14725,7 +14725,7 @@
         <v>128</v>
       </c>
       <c r="V201" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="202" spans="1:22" x14ac:dyDescent="0.2">
@@ -14793,7 +14793,7 @@
         <v>128</v>
       </c>
       <c r="V202" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="203" spans="1:22" x14ac:dyDescent="0.2">
@@ -14861,7 +14861,7 @@
         <v>128</v>
       </c>
       <c r="V203" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="204" spans="1:22" x14ac:dyDescent="0.2">
@@ -14929,7 +14929,7 @@
         <v>128</v>
       </c>
       <c r="V204" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="205" spans="1:22" x14ac:dyDescent="0.2">
@@ -14997,7 +14997,7 @@
         <v>128</v>
       </c>
       <c r="V205" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="206" spans="1:22" x14ac:dyDescent="0.2">
@@ -15065,7 +15065,7 @@
         <v>128</v>
       </c>
       <c r="V206" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="207" spans="1:22" x14ac:dyDescent="0.2">
@@ -15133,7 +15133,7 @@
         <v>128</v>
       </c>
       <c r="V207" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="208" spans="1:22" x14ac:dyDescent="0.2">
@@ -15201,7 +15201,7 @@
         <v>128</v>
       </c>
       <c r="V208" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="209" spans="1:22" x14ac:dyDescent="0.2">
@@ -15269,7 +15269,7 @@
         <v>128</v>
       </c>
       <c r="V209" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="210" spans="1:22" x14ac:dyDescent="0.2">
@@ -15337,7 +15337,7 @@
         <v>128</v>
       </c>
       <c r="V210" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="211" spans="1:22" x14ac:dyDescent="0.2">
@@ -15405,7 +15405,7 @@
         <v>128</v>
       </c>
       <c r="V211" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="212" spans="1:22" x14ac:dyDescent="0.2">
@@ -15473,7 +15473,7 @@
         <v>128</v>
       </c>
       <c r="V212" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="213" spans="1:22" x14ac:dyDescent="0.2">
@@ -15541,7 +15541,7 @@
         <v>128</v>
       </c>
       <c r="V213" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="214" spans="1:22" x14ac:dyDescent="0.2">
@@ -15609,7 +15609,7 @@
         <v>128</v>
       </c>
       <c r="V214" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="215" spans="1:22" x14ac:dyDescent="0.2">
@@ -15677,7 +15677,7 @@
         <v>128</v>
       </c>
       <c r="V215" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="216" spans="1:22" x14ac:dyDescent="0.2">
@@ -15745,7 +15745,7 @@
         <v>128</v>
       </c>
       <c r="V216" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="217" spans="1:22" x14ac:dyDescent="0.2">
@@ -15813,7 +15813,7 @@
         <v>128</v>
       </c>
       <c r="V217" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="218" spans="1:22" x14ac:dyDescent="0.2">
@@ -15881,7 +15881,7 @@
         <v>128</v>
       </c>
       <c r="V218" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="219" spans="1:22" x14ac:dyDescent="0.2">
@@ -15949,7 +15949,7 @@
         <v>128</v>
       </c>
       <c r="V219" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="220" spans="1:22" x14ac:dyDescent="0.2">
@@ -16017,7 +16017,7 @@
         <v>128</v>
       </c>
       <c r="V220" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="221" spans="1:22" x14ac:dyDescent="0.2">
@@ -16085,7 +16085,7 @@
         <v>128</v>
       </c>
       <c r="V221" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="222" spans="1:22" x14ac:dyDescent="0.2">
@@ -16153,7 +16153,7 @@
         <v>128</v>
       </c>
       <c r="V222" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="223" spans="1:22" x14ac:dyDescent="0.2">
@@ -16221,7 +16221,7 @@
         <v>128</v>
       </c>
       <c r="V223" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="224" spans="1:22" x14ac:dyDescent="0.2">
@@ -16289,7 +16289,7 @@
         <v>128</v>
       </c>
       <c r="V224" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="225" spans="1:22" x14ac:dyDescent="0.2">
@@ -16357,7 +16357,7 @@
         <v>128</v>
       </c>
       <c r="V225" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="226" spans="1:22" x14ac:dyDescent="0.2">
@@ -16425,7 +16425,7 @@
         <v>128</v>
       </c>
       <c r="V226" s="17" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="227" spans="1:22" x14ac:dyDescent="0.2">
@@ -18326,10 +18326,10 @@
         <v>96</v>
       </c>
       <c r="U254" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V254" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="255" spans="1:22" x14ac:dyDescent="0.2">
@@ -18394,10 +18394,10 @@
         <v>96</v>
       </c>
       <c r="U255" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V255" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="256" spans="1:22" x14ac:dyDescent="0.2">
@@ -18462,10 +18462,10 @@
         <v>96</v>
       </c>
       <c r="U256" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V256" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="257" spans="1:22" x14ac:dyDescent="0.2">
@@ -18530,10 +18530,10 @@
         <v>96</v>
       </c>
       <c r="U257" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V257" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="258" spans="1:22" x14ac:dyDescent="0.2">
@@ -18598,10 +18598,10 @@
         <v>96</v>
       </c>
       <c r="U258" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V258" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="259" spans="1:22" x14ac:dyDescent="0.2">
@@ -18666,10 +18666,10 @@
         <v>96</v>
       </c>
       <c r="U259" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V259" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="260" spans="1:22" x14ac:dyDescent="0.2">
@@ -18734,10 +18734,10 @@
         <v>96</v>
       </c>
       <c r="U260" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V260" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="261" spans="1:22" x14ac:dyDescent="0.2">
@@ -18802,10 +18802,10 @@
         <v>96</v>
       </c>
       <c r="U261" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V261" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="262" spans="1:22" x14ac:dyDescent="0.2">
@@ -18870,10 +18870,10 @@
         <v>96</v>
       </c>
       <c r="U262" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V262" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="263" spans="1:22" x14ac:dyDescent="0.2">
@@ -18938,10 +18938,10 @@
         <v>96</v>
       </c>
       <c r="U263" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V263" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="264" spans="1:22" x14ac:dyDescent="0.2">
@@ -19006,10 +19006,10 @@
         <v>96</v>
       </c>
       <c r="U264" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V264" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="265" spans="1:22" x14ac:dyDescent="0.2">
@@ -19074,10 +19074,10 @@
         <v>96</v>
       </c>
       <c r="U265" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V265" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="266" spans="1:22" x14ac:dyDescent="0.2">
@@ -19142,10 +19142,10 @@
         <v>96</v>
       </c>
       <c r="U266" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V266" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="267" spans="1:22" x14ac:dyDescent="0.2">
@@ -19210,10 +19210,10 @@
         <v>96</v>
       </c>
       <c r="U267" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V267" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="268" spans="1:22" x14ac:dyDescent="0.2">
@@ -19278,10 +19278,10 @@
         <v>96</v>
       </c>
       <c r="U268" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V268" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="269" spans="1:22" x14ac:dyDescent="0.2">
@@ -19346,10 +19346,10 @@
         <v>96</v>
       </c>
       <c r="U269" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V269" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="270" spans="1:22" x14ac:dyDescent="0.2">
@@ -19417,7 +19417,7 @@
         <v>157</v>
       </c>
       <c r="V270" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="271" spans="1:22" x14ac:dyDescent="0.2">
@@ -19485,7 +19485,7 @@
         <v>157</v>
       </c>
       <c r="V271" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="272" spans="1:22" x14ac:dyDescent="0.2">
@@ -19553,7 +19553,7 @@
         <v>157</v>
       </c>
       <c r="V272" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="273" spans="1:22" x14ac:dyDescent="0.2">
@@ -19621,7 +19621,7 @@
         <v>157</v>
       </c>
       <c r="V273" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="274" spans="1:22" x14ac:dyDescent="0.2">
@@ -19689,7 +19689,7 @@
         <v>157</v>
       </c>
       <c r="V274" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="275" spans="1:22" x14ac:dyDescent="0.2">
@@ -19757,7 +19757,7 @@
         <v>157</v>
       </c>
       <c r="V275" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="276" spans="1:22" x14ac:dyDescent="0.2">
@@ -19825,7 +19825,7 @@
         <v>157</v>
       </c>
       <c r="V276" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="277" spans="1:22" x14ac:dyDescent="0.2">
@@ -19893,7 +19893,7 @@
         <v>157</v>
       </c>
       <c r="V277" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="278" spans="1:22" x14ac:dyDescent="0.2">
@@ -19961,7 +19961,7 @@
         <v>157</v>
       </c>
       <c r="V278" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="279" spans="1:22" x14ac:dyDescent="0.2">
@@ -20029,7 +20029,7 @@
         <v>157</v>
       </c>
       <c r="V279" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="280" spans="1:22" x14ac:dyDescent="0.2">
@@ -20097,7 +20097,7 @@
         <v>157</v>
       </c>
       <c r="V280" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="281" spans="1:22" x14ac:dyDescent="0.2">
@@ -20165,7 +20165,7 @@
         <v>157</v>
       </c>
       <c r="V281" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="282" spans="1:22" x14ac:dyDescent="0.2">
@@ -20233,7 +20233,7 @@
         <v>157</v>
       </c>
       <c r="V282" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="283" spans="1:22" x14ac:dyDescent="0.2">
@@ -20301,7 +20301,7 @@
         <v>157</v>
       </c>
       <c r="V283" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="284" spans="1:22" x14ac:dyDescent="0.2">
@@ -20369,7 +20369,7 @@
         <v>157</v>
       </c>
       <c r="V284" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="285" spans="1:22" x14ac:dyDescent="0.2">
@@ -20437,7 +20437,7 @@
         <v>157</v>
       </c>
       <c r="V285" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="286" spans="1:22" x14ac:dyDescent="0.2">
@@ -20505,7 +20505,7 @@
         <v>157</v>
       </c>
       <c r="V286" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="287" spans="1:22" x14ac:dyDescent="0.2">
@@ -20573,7 +20573,7 @@
         <v>157</v>
       </c>
       <c r="V287" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="288" spans="1:22" x14ac:dyDescent="0.2">
@@ -20641,7 +20641,7 @@
         <v>157</v>
       </c>
       <c r="V288" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="289" spans="1:22" x14ac:dyDescent="0.2">
@@ -20709,7 +20709,7 @@
         <v>157</v>
       </c>
       <c r="V289" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="290" spans="1:22" x14ac:dyDescent="0.2">
@@ -20777,7 +20777,7 @@
         <v>157</v>
       </c>
       <c r="V290" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="291" spans="1:22" x14ac:dyDescent="0.2">
@@ -20845,7 +20845,7 @@
         <v>157</v>
       </c>
       <c r="V291" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="292" spans="1:22" x14ac:dyDescent="0.2">
@@ -20913,7 +20913,7 @@
         <v>157</v>
       </c>
       <c r="V292" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="293" spans="1:22" x14ac:dyDescent="0.2">
@@ -20981,7 +20981,7 @@
         <v>157</v>
       </c>
       <c r="V293" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="294" spans="1:22" x14ac:dyDescent="0.2">
@@ -21049,7 +21049,7 @@
         <v>157</v>
       </c>
       <c r="V294" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="295" spans="1:22" x14ac:dyDescent="0.2">
@@ -21117,7 +21117,7 @@
         <v>157</v>
       </c>
       <c r="V295" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="296" spans="1:22" x14ac:dyDescent="0.2">
@@ -21185,7 +21185,7 @@
         <v>157</v>
       </c>
       <c r="V296" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="297" spans="1:22" x14ac:dyDescent="0.2">
@@ -21253,7 +21253,7 @@
         <v>157</v>
       </c>
       <c r="V297" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="298" spans="1:22" x14ac:dyDescent="0.2">
@@ -21321,7 +21321,7 @@
         <v>157</v>
       </c>
       <c r="V298" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="299" spans="1:22" x14ac:dyDescent="0.2">
@@ -21389,7 +21389,7 @@
         <v>157</v>
       </c>
       <c r="V299" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="300" spans="1:22" x14ac:dyDescent="0.2">
@@ -29377,7 +29377,7 @@
         <v>128</v>
       </c>
       <c r="V420" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="421" spans="1:22" x14ac:dyDescent="0.2">
@@ -29445,7 +29445,7 @@
         <v>128</v>
       </c>
       <c r="V421" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="422" spans="1:22" x14ac:dyDescent="0.2">
@@ -29513,7 +29513,7 @@
         <v>128</v>
       </c>
       <c r="V422" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="423" spans="1:22" x14ac:dyDescent="0.2">
@@ -29581,7 +29581,7 @@
         <v>128</v>
       </c>
       <c r="V423" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="424" spans="1:22" x14ac:dyDescent="0.2">
@@ -29649,7 +29649,7 @@
         <v>128</v>
       </c>
       <c r="V424" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="425" spans="1:22" x14ac:dyDescent="0.2">
@@ -29717,7 +29717,7 @@
         <v>128</v>
       </c>
       <c r="V425" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="426" spans="1:22" x14ac:dyDescent="0.2">
@@ -29785,7 +29785,7 @@
         <v>128</v>
       </c>
       <c r="V426" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="427" spans="1:22" x14ac:dyDescent="0.2">
@@ -29853,7 +29853,7 @@
         <v>128</v>
       </c>
       <c r="V427" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="428" spans="1:22" x14ac:dyDescent="0.2">
@@ -29921,7 +29921,7 @@
         <v>128</v>
       </c>
       <c r="V428" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="429" spans="1:22" x14ac:dyDescent="0.2">
@@ -29989,7 +29989,7 @@
         <v>128</v>
       </c>
       <c r="V429" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="430" spans="1:22" x14ac:dyDescent="0.2">
@@ -30057,7 +30057,7 @@
         <v>128</v>
       </c>
       <c r="V430" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="431" spans="1:22" x14ac:dyDescent="0.2">
@@ -30125,7 +30125,7 @@
         <v>128</v>
       </c>
       <c r="V431" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="432" spans="1:22" x14ac:dyDescent="0.2">
@@ -30193,7 +30193,7 @@
         <v>128</v>
       </c>
       <c r="V432" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="433" spans="1:22" x14ac:dyDescent="0.2">
@@ -30261,7 +30261,7 @@
         <v>128</v>
       </c>
       <c r="V433" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="434" spans="1:22" x14ac:dyDescent="0.2">
@@ -30329,7 +30329,7 @@
         <v>128</v>
       </c>
       <c r="V434" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="435" spans="1:22" x14ac:dyDescent="0.2">
@@ -30397,7 +30397,7 @@
         <v>128</v>
       </c>
       <c r="V435" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="436" spans="1:22" x14ac:dyDescent="0.2">
@@ -30465,7 +30465,7 @@
         <v>128</v>
       </c>
       <c r="V436" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="437" spans="1:22" x14ac:dyDescent="0.2">
@@ -30533,7 +30533,7 @@
         <v>128</v>
       </c>
       <c r="V437" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="438" spans="1:22" x14ac:dyDescent="0.2">
@@ -30601,7 +30601,7 @@
         <v>128</v>
       </c>
       <c r="V438" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="439" spans="1:22" x14ac:dyDescent="0.2">
@@ -30669,7 +30669,7 @@
         <v>128</v>
       </c>
       <c r="V439" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="440" spans="1:22" x14ac:dyDescent="0.2">
@@ -30737,7 +30737,7 @@
         <v>128</v>
       </c>
       <c r="V440" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="441" spans="1:22" x14ac:dyDescent="0.2">
@@ -30805,7 +30805,7 @@
         <v>128</v>
       </c>
       <c r="V441" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="442" spans="1:22" x14ac:dyDescent="0.2">
@@ -30873,7 +30873,7 @@
         <v>128</v>
       </c>
       <c r="V442" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="443" spans="1:22" x14ac:dyDescent="0.2">
@@ -30941,7 +30941,7 @@
         <v>128</v>
       </c>
       <c r="V443" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="444" spans="1:22" x14ac:dyDescent="0.2">
@@ -31009,7 +31009,7 @@
         <v>128</v>
       </c>
       <c r="V444" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="445" spans="1:22" x14ac:dyDescent="0.2">
@@ -31077,7 +31077,7 @@
         <v>128</v>
       </c>
       <c r="V445" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="446" spans="1:22" x14ac:dyDescent="0.2">
@@ -31145,7 +31145,7 @@
         <v>128</v>
       </c>
       <c r="V446" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="447" spans="1:22" x14ac:dyDescent="0.2">
@@ -31213,7 +31213,7 @@
         <v>128</v>
       </c>
       <c r="V447" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="448" spans="1:22" x14ac:dyDescent="0.2">
@@ -31281,7 +31281,7 @@
         <v>128</v>
       </c>
       <c r="V448" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="449" spans="1:22" x14ac:dyDescent="0.2">
@@ -31349,7 +31349,7 @@
         <v>128</v>
       </c>
       <c r="V449" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="450" spans="1:22" x14ac:dyDescent="0.2">
@@ -31417,7 +31417,7 @@
         <v>128</v>
       </c>
       <c r="V450" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="451" spans="1:22" x14ac:dyDescent="0.2">
@@ -31485,7 +31485,7 @@
         <v>128</v>
       </c>
       <c r="V451" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="452" spans="1:22" x14ac:dyDescent="0.2">
@@ -31553,7 +31553,7 @@
         <v>128</v>
       </c>
       <c r="V452" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="453" spans="1:22" x14ac:dyDescent="0.2">
@@ -31621,7 +31621,7 @@
         <v>128</v>
       </c>
       <c r="V453" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="454" spans="1:22" x14ac:dyDescent="0.2">
@@ -31689,7 +31689,7 @@
         <v>128</v>
       </c>
       <c r="V454" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="455" spans="1:22" x14ac:dyDescent="0.2">
@@ -31757,7 +31757,7 @@
         <v>128</v>
       </c>
       <c r="V455" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="456" spans="1:22" x14ac:dyDescent="0.2">
@@ -31825,7 +31825,7 @@
         <v>128</v>
       </c>
       <c r="V456" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="457" spans="1:22" x14ac:dyDescent="0.2">
@@ -31893,7 +31893,7 @@
         <v>128</v>
       </c>
       <c r="V457" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="458" spans="1:22" x14ac:dyDescent="0.2">
@@ -31961,7 +31961,7 @@
         <v>128</v>
       </c>
       <c r="V458" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="459" spans="1:22" x14ac:dyDescent="0.2">
@@ -32029,7 +32029,7 @@
         <v>128</v>
       </c>
       <c r="V459" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="460" spans="1:22" x14ac:dyDescent="0.2">
@@ -32097,7 +32097,7 @@
         <v>128</v>
       </c>
       <c r="V460" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="461" spans="1:22" x14ac:dyDescent="0.2">
@@ -32165,7 +32165,7 @@
         <v>128</v>
       </c>
       <c r="V461" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="462" spans="1:22" x14ac:dyDescent="0.2">
@@ -32233,7 +32233,7 @@
         <v>128</v>
       </c>
       <c r="V462" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="463" spans="1:22" x14ac:dyDescent="0.2">
@@ -32301,7 +32301,7 @@
         <v>128</v>
       </c>
       <c r="V463" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="464" spans="1:22" x14ac:dyDescent="0.2">
@@ -32369,7 +32369,7 @@
         <v>128</v>
       </c>
       <c r="V464" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="465" spans="1:22" x14ac:dyDescent="0.2">
@@ -32437,7 +32437,7 @@
         <v>128</v>
       </c>
       <c r="V465" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="466" spans="1:22" x14ac:dyDescent="0.2">
@@ -32505,7 +32505,7 @@
         <v>128</v>
       </c>
       <c r="V466" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="467" spans="1:22" x14ac:dyDescent="0.2">
@@ -32573,7 +32573,7 @@
         <v>128</v>
       </c>
       <c r="V467" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="468" spans="1:22" x14ac:dyDescent="0.2">
@@ -32641,7 +32641,7 @@
         <v>128</v>
       </c>
       <c r="V468" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="469" spans="1:22" x14ac:dyDescent="0.2">
@@ -32709,7 +32709,7 @@
         <v>128</v>
       </c>
       <c r="V469" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="470" spans="1:22" x14ac:dyDescent="0.2">
@@ -32777,7 +32777,7 @@
         <v>128</v>
       </c>
       <c r="V470" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="471" spans="1:22" x14ac:dyDescent="0.2">
@@ -32845,7 +32845,7 @@
         <v>128</v>
       </c>
       <c r="V471" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="472" spans="1:22" x14ac:dyDescent="0.2">
@@ -32913,7 +32913,7 @@
         <v>128</v>
       </c>
       <c r="V472" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="473" spans="1:22" x14ac:dyDescent="0.2">
@@ -32981,7 +32981,7 @@
         <v>128</v>
       </c>
       <c r="V473" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="474" spans="1:22" x14ac:dyDescent="0.2">
@@ -33049,7 +33049,7 @@
         <v>128</v>
       </c>
       <c r="V474" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="475" spans="1:22" x14ac:dyDescent="0.2">
@@ -33117,7 +33117,7 @@
         <v>128</v>
       </c>
       <c r="V475" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="476" spans="1:22" x14ac:dyDescent="0.2">
@@ -33185,7 +33185,7 @@
         <v>128</v>
       </c>
       <c r="V476" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="477" spans="1:22" x14ac:dyDescent="0.2">
@@ -33253,7 +33253,7 @@
         <v>128</v>
       </c>
       <c r="V477" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="478" spans="1:22" x14ac:dyDescent="0.2">
@@ -33321,7 +33321,7 @@
         <v>128</v>
       </c>
       <c r="V478" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="479" spans="1:22" x14ac:dyDescent="0.2">
@@ -33389,7 +33389,7 @@
         <v>128</v>
       </c>
       <c r="V479" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="480" spans="1:22" x14ac:dyDescent="0.2">
@@ -33457,7 +33457,7 @@
         <v>128</v>
       </c>
       <c r="V480" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="481" spans="1:22" x14ac:dyDescent="0.2">
@@ -33525,7 +33525,7 @@
         <v>128</v>
       </c>
       <c r="V481" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="482" spans="1:22" x14ac:dyDescent="0.2">
@@ -33593,7 +33593,7 @@
         <v>128</v>
       </c>
       <c r="V482" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="483" spans="1:22" x14ac:dyDescent="0.2">
@@ -33661,7 +33661,7 @@
         <v>128</v>
       </c>
       <c r="V483" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="484" spans="1:22" x14ac:dyDescent="0.2">
@@ -33729,7 +33729,7 @@
         <v>128</v>
       </c>
       <c r="V484" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="485" spans="1:22" x14ac:dyDescent="0.2">
@@ -33797,7 +33797,7 @@
         <v>128</v>
       </c>
       <c r="V485" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="486" spans="1:22" x14ac:dyDescent="0.2">
@@ -33865,7 +33865,7 @@
         <v>128</v>
       </c>
       <c r="V486" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="487" spans="1:22" x14ac:dyDescent="0.2">
@@ -33933,7 +33933,7 @@
         <v>128</v>
       </c>
       <c r="V487" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="488" spans="1:22" x14ac:dyDescent="0.2">
@@ -34001,7 +34001,7 @@
         <v>128</v>
       </c>
       <c r="V488" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="489" spans="1:22" x14ac:dyDescent="0.2">
@@ -34069,7 +34069,7 @@
         <v>128</v>
       </c>
       <c r="V489" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="490" spans="1:22" x14ac:dyDescent="0.2">
@@ -34134,10 +34134,10 @@
         <v>11.2</v>
       </c>
       <c r="U490" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V490" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="491" spans="1:22" x14ac:dyDescent="0.2">
@@ -34202,10 +34202,10 @@
         <v>11.2</v>
       </c>
       <c r="U491" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V491" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="492" spans="1:22" x14ac:dyDescent="0.2">
@@ -34270,10 +34270,10 @@
         <v>11.2</v>
       </c>
       <c r="U492" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V492" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="493" spans="1:22" x14ac:dyDescent="0.2">
@@ -34338,10 +34338,10 @@
         <v>11.2</v>
       </c>
       <c r="U493" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V493" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="494" spans="1:22" x14ac:dyDescent="0.2">
@@ -34406,10 +34406,10 @@
         <v>11.2</v>
       </c>
       <c r="U494" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V494" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="495" spans="1:22" x14ac:dyDescent="0.2">
@@ -34474,10 +34474,10 @@
         <v>11.2</v>
       </c>
       <c r="U495" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V495" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="496" spans="1:22" x14ac:dyDescent="0.2">
@@ -34542,10 +34542,10 @@
         <v>11.2</v>
       </c>
       <c r="U496" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V496" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="497" spans="1:22" x14ac:dyDescent="0.2">
@@ -34610,10 +34610,10 @@
         <v>11.2</v>
       </c>
       <c r="U497" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V497" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="498" spans="1:22" x14ac:dyDescent="0.2">
@@ -34678,10 +34678,10 @@
         <v>11.2</v>
       </c>
       <c r="U498" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V498" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="499" spans="1:22" x14ac:dyDescent="0.2">
@@ -34746,10 +34746,10 @@
         <v>11.2</v>
       </c>
       <c r="U499" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V499" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="500" spans="1:22" x14ac:dyDescent="0.2">
@@ -34814,10 +34814,10 @@
         <v>11.2</v>
       </c>
       <c r="U500" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V500" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="501" spans="1:22" x14ac:dyDescent="0.2">
@@ -34882,10 +34882,10 @@
         <v>11.2</v>
       </c>
       <c r="U501" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V501" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="502" spans="1:22" x14ac:dyDescent="0.2">
@@ -34950,10 +34950,10 @@
         <v>11.2</v>
       </c>
       <c r="U502" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V502" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="503" spans="1:22" x14ac:dyDescent="0.2">
@@ -35018,10 +35018,10 @@
         <v>11.2</v>
       </c>
       <c r="U503" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V503" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="504" spans="1:22" x14ac:dyDescent="0.2">
@@ -35086,10 +35086,10 @@
         <v>11.2</v>
       </c>
       <c r="U504" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V504" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="505" spans="1:22" x14ac:dyDescent="0.2">
@@ -35154,10 +35154,10 @@
         <v>11.2</v>
       </c>
       <c r="U505" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V505" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="506" spans="1:22" x14ac:dyDescent="0.2">
@@ -35222,10 +35222,10 @@
         <v>11.2</v>
       </c>
       <c r="U506" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V506" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="507" spans="1:22" x14ac:dyDescent="0.2">
@@ -35290,10 +35290,10 @@
         <v>11.2</v>
       </c>
       <c r="U507" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V507" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="508" spans="1:22" x14ac:dyDescent="0.2">
@@ -35358,10 +35358,10 @@
         <v>11.2</v>
       </c>
       <c r="U508" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V508" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="509" spans="1:22" x14ac:dyDescent="0.2">
@@ -35426,10 +35426,10 @@
         <v>11.2</v>
       </c>
       <c r="U509" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V509" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="510" spans="1:22" x14ac:dyDescent="0.2">
@@ -35494,10 +35494,10 @@
         <v>11.2</v>
       </c>
       <c r="U510" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V510" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="511" spans="1:22" x14ac:dyDescent="0.2">
@@ -35562,10 +35562,10 @@
         <v>11.2</v>
       </c>
       <c r="U511" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V511" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="512" spans="1:22" x14ac:dyDescent="0.2">
@@ -35630,10 +35630,10 @@
         <v>11.2</v>
       </c>
       <c r="U512" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V512" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="513" spans="1:22" x14ac:dyDescent="0.2">
@@ -35698,10 +35698,10 @@
         <v>11.2</v>
       </c>
       <c r="U513" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V513" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="514" spans="1:22" x14ac:dyDescent="0.2">
@@ -38604,10 +38604,10 @@
         <v>16.8</v>
       </c>
       <c r="U557" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V557" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="558" spans="1:22" x14ac:dyDescent="0.2">
@@ -38672,10 +38672,10 @@
         <v>16.8</v>
       </c>
       <c r="U558" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V558" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="559" spans="1:22" x14ac:dyDescent="0.2">
@@ -38740,10 +38740,10 @@
         <v>16.8</v>
       </c>
       <c r="U559" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V559" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="560" spans="1:22" x14ac:dyDescent="0.2">
@@ -38808,10 +38808,10 @@
         <v>16.8</v>
       </c>
       <c r="U560" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V560" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="561" spans="1:22" x14ac:dyDescent="0.2">
@@ -38876,10 +38876,10 @@
         <v>16.8</v>
       </c>
       <c r="U561" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V561" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="562" spans="1:22" x14ac:dyDescent="0.2">
@@ -38944,10 +38944,10 @@
         <v>16.8</v>
       </c>
       <c r="U562" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V562" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="563" spans="1:22" x14ac:dyDescent="0.2">
@@ -39012,10 +39012,10 @@
         <v>16.8</v>
       </c>
       <c r="U563" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V563" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="564" spans="1:22" x14ac:dyDescent="0.2">
@@ -39080,10 +39080,10 @@
         <v>16.8</v>
       </c>
       <c r="U564" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V564" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="565" spans="1:22" x14ac:dyDescent="0.2">
@@ -39148,10 +39148,10 @@
         <v>16.8</v>
       </c>
       <c r="U565" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V565" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="566" spans="1:22" x14ac:dyDescent="0.2">
@@ -39216,10 +39216,10 @@
         <v>16.8</v>
       </c>
       <c r="U566" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V566" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="567" spans="1:22" x14ac:dyDescent="0.2">
@@ -39284,10 +39284,10 @@
         <v>16.8</v>
       </c>
       <c r="U567" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V567" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="568" spans="1:22" x14ac:dyDescent="0.2">
@@ -39352,10 +39352,10 @@
         <v>16.8</v>
       </c>
       <c r="U568" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V568" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="569" spans="1:22" x14ac:dyDescent="0.2">
@@ -39420,10 +39420,10 @@
         <v>16.8</v>
       </c>
       <c r="U569" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V569" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="570" spans="1:22" x14ac:dyDescent="0.2">
@@ -39488,10 +39488,10 @@
         <v>16.8</v>
       </c>
       <c r="U570" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V570" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="571" spans="1:22" x14ac:dyDescent="0.2">
@@ -39556,10 +39556,10 @@
         <v>16.8</v>
       </c>
       <c r="U571" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V571" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="572" spans="1:22" x14ac:dyDescent="0.2">
@@ -39624,10 +39624,10 @@
         <v>16.8</v>
       </c>
       <c r="U572" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V572" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="573" spans="1:22" x14ac:dyDescent="0.2">
@@ -39692,10 +39692,10 @@
         <v>16.8</v>
       </c>
       <c r="U573" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V573" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="574" spans="1:22" x14ac:dyDescent="0.2">
@@ -39760,10 +39760,10 @@
         <v>16.8</v>
       </c>
       <c r="U574" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V574" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="575" spans="1:22" x14ac:dyDescent="0.2">
@@ -39828,10 +39828,10 @@
         <v>16.8</v>
       </c>
       <c r="U575" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V575" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="576" spans="1:22" x14ac:dyDescent="0.2">
@@ -39896,10 +39896,10 @@
         <v>16.8</v>
       </c>
       <c r="U576" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V576" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="577" spans="1:22" x14ac:dyDescent="0.2">
@@ -39964,10 +39964,10 @@
         <v>26.8</v>
       </c>
       <c r="U577" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V577" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V577" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="578" spans="1:22" x14ac:dyDescent="0.2">
@@ -40032,10 +40032,10 @@
         <v>26.8</v>
       </c>
       <c r="U578" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V578" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V578" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="579" spans="1:22" x14ac:dyDescent="0.2">
@@ -40100,10 +40100,10 @@
         <v>26.8</v>
       </c>
       <c r="U579" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V579" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V579" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="580" spans="1:22" x14ac:dyDescent="0.2">
@@ -40168,10 +40168,10 @@
         <v>26.8</v>
       </c>
       <c r="U580" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V580" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V580" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="581" spans="1:22" x14ac:dyDescent="0.2">
@@ -40236,10 +40236,10 @@
         <v>26.8</v>
       </c>
       <c r="U581" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V581" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V581" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="582" spans="1:22" x14ac:dyDescent="0.2">
@@ -40304,10 +40304,10 @@
         <v>26.8</v>
       </c>
       <c r="U582" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V582" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V582" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="583" spans="1:22" x14ac:dyDescent="0.2">
@@ -40372,10 +40372,10 @@
         <v>26.8</v>
       </c>
       <c r="U583" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V583" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V583" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="584" spans="1:22" x14ac:dyDescent="0.2">
@@ -40440,10 +40440,10 @@
         <v>26.8</v>
       </c>
       <c r="U584" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V584" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V584" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="585" spans="1:22" x14ac:dyDescent="0.2">
@@ -40508,10 +40508,10 @@
         <v>26.8</v>
       </c>
       <c r="U585" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V585" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V585" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="586" spans="1:22" x14ac:dyDescent="0.2">
@@ -40576,10 +40576,10 @@
         <v>26.8</v>
       </c>
       <c r="U586" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V586" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V586" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="587" spans="1:22" x14ac:dyDescent="0.2">
@@ -40644,10 +40644,10 @@
         <v>26.8</v>
       </c>
       <c r="U587" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V587" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V587" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="588" spans="1:22" x14ac:dyDescent="0.2">
@@ -40712,10 +40712,10 @@
         <v>26.8</v>
       </c>
       <c r="U588" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V588" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V588" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="589" spans="1:22" x14ac:dyDescent="0.2">
@@ -40780,10 +40780,10 @@
         <v>26.8</v>
       </c>
       <c r="U589" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V589" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V589" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="590" spans="1:22" x14ac:dyDescent="0.2">
@@ -40848,10 +40848,10 @@
         <v>26.8</v>
       </c>
       <c r="U590" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V590" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V590" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="591" spans="1:22" x14ac:dyDescent="0.2">
@@ -40916,10 +40916,10 @@
         <v>26.8</v>
       </c>
       <c r="U591" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V591" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V591" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="592" spans="1:22" x14ac:dyDescent="0.2">
@@ -40984,10 +40984,10 @@
         <v>26.8</v>
       </c>
       <c r="U592" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V592" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V592" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="593" spans="1:22" x14ac:dyDescent="0.2">
@@ -41052,10 +41052,10 @@
         <v>26.8</v>
       </c>
       <c r="U593" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V593" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V593" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="594" spans="1:22" x14ac:dyDescent="0.2">
@@ -41120,10 +41120,10 @@
         <v>26.8</v>
       </c>
       <c r="U594" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V594" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V594" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="595" spans="1:22" x14ac:dyDescent="0.2">
@@ -41188,10 +41188,10 @@
         <v>26.8</v>
       </c>
       <c r="U595" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V595" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V595" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="596" spans="1:22" x14ac:dyDescent="0.2">
@@ -41256,10 +41256,10 @@
         <v>26.8</v>
       </c>
       <c r="U596" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V596" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V596" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="597" spans="1:22" x14ac:dyDescent="0.2">
@@ -41324,10 +41324,10 @@
         <v>26.8</v>
       </c>
       <c r="U597" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V597" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V597" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="598" spans="1:22" x14ac:dyDescent="0.2">
@@ -41392,10 +41392,10 @@
         <v>26.8</v>
       </c>
       <c r="U598" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V598" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V598" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="599" spans="1:22" x14ac:dyDescent="0.2">
@@ -41460,10 +41460,10 @@
         <v>26.8</v>
       </c>
       <c r="U599" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V599" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V599" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="600" spans="1:22" x14ac:dyDescent="0.2">
@@ -41528,10 +41528,10 @@
         <v>26.8</v>
       </c>
       <c r="U600" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V600" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V600" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="601" spans="1:22" x14ac:dyDescent="0.2">
@@ -41596,10 +41596,10 @@
         <v>26.8</v>
       </c>
       <c r="U601" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V601" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V601" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="602" spans="1:22" x14ac:dyDescent="0.2">
@@ -41664,10 +41664,10 @@
         <v>26.8</v>
       </c>
       <c r="U602" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V602" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V602" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="603" spans="1:22" x14ac:dyDescent="0.2">
@@ -41732,10 +41732,10 @@
         <v>26.8</v>
       </c>
       <c r="U603" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V603" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V603" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="604" spans="1:22" x14ac:dyDescent="0.2">
@@ -41800,10 +41800,10 @@
         <v>26.8</v>
       </c>
       <c r="U604" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V604" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V604" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="605" spans="1:22" x14ac:dyDescent="0.2">
@@ -41868,10 +41868,10 @@
         <v>26.8</v>
       </c>
       <c r="U605" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V605" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V605" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="606" spans="1:22" x14ac:dyDescent="0.2">
@@ -41936,10 +41936,10 @@
         <v>26.8</v>
       </c>
       <c r="U606" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V606" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V606" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="607" spans="1:22" x14ac:dyDescent="0.2">
@@ -42004,10 +42004,10 @@
         <v>26.8</v>
       </c>
       <c r="U607" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V607" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V607" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="608" spans="1:22" x14ac:dyDescent="0.2">
@@ -42072,10 +42072,10 @@
         <v>26.8</v>
       </c>
       <c r="U608" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V608" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V608" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="609" spans="1:22" x14ac:dyDescent="0.2">
@@ -42140,10 +42140,10 @@
         <v>26.8</v>
       </c>
       <c r="U609" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V609" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V609" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="610" spans="1:22" x14ac:dyDescent="0.2">
@@ -42208,10 +42208,10 @@
         <v>26.8</v>
       </c>
       <c r="U610" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V610" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V610" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="611" spans="1:22" x14ac:dyDescent="0.2">
@@ -42276,10 +42276,10 @@
         <v>26.8</v>
       </c>
       <c r="U611" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V611" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V611" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="612" spans="1:22" x14ac:dyDescent="0.2">
@@ -42344,10 +42344,10 @@
         <v>26.8</v>
       </c>
       <c r="U612" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V612" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V612" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="613" spans="1:22" x14ac:dyDescent="0.2">
@@ -42412,10 +42412,10 @@
         <v>26.8</v>
       </c>
       <c r="U613" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V613" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V613" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="614" spans="1:22" x14ac:dyDescent="0.2">
@@ -42480,10 +42480,10 @@
         <v>26.8</v>
       </c>
       <c r="U614" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V614" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V614" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="615" spans="1:22" x14ac:dyDescent="0.2">
@@ -42548,10 +42548,10 @@
         <v>26.8</v>
       </c>
       <c r="U615" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V615" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V615" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="616" spans="1:22" x14ac:dyDescent="0.2">
@@ -42616,10 +42616,10 @@
         <v>26.8</v>
       </c>
       <c r="U616" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V616" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V616" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="617" spans="1:22" x14ac:dyDescent="0.2">
@@ -42684,10 +42684,10 @@
         <v>26.8</v>
       </c>
       <c r="U617" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V617" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V617" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="618" spans="1:22" x14ac:dyDescent="0.2">
@@ -42752,10 +42752,10 @@
         <v>26.8</v>
       </c>
       <c r="U618" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V618" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V618" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="619" spans="1:22" x14ac:dyDescent="0.2">
@@ -42820,10 +42820,10 @@
         <v>26.8</v>
       </c>
       <c r="U619" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V619" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V619" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="620" spans="1:22" x14ac:dyDescent="0.2">
@@ -42888,10 +42888,10 @@
         <v>26.8</v>
       </c>
       <c r="U620" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V620" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V620" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="621" spans="1:22" x14ac:dyDescent="0.2">
@@ -42956,10 +42956,10 @@
         <v>26.8</v>
       </c>
       <c r="U621" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V621" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V621" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="622" spans="1:22" x14ac:dyDescent="0.2">
@@ -43024,10 +43024,10 @@
         <v>26.8</v>
       </c>
       <c r="U622" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V622" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V622" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="623" spans="1:22" x14ac:dyDescent="0.2">
@@ -43092,10 +43092,10 @@
         <v>26.8</v>
       </c>
       <c r="U623" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V623" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V623" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="624" spans="1:22" x14ac:dyDescent="0.2">
@@ -43160,10 +43160,10 @@
         <v>26.8</v>
       </c>
       <c r="U624" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V624" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V624" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="625" spans="1:22" x14ac:dyDescent="0.2">
@@ -43228,10 +43228,10 @@
         <v>26.8</v>
       </c>
       <c r="U625" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V625" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V625" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="626" spans="1:22" x14ac:dyDescent="0.2">
@@ -43296,10 +43296,10 @@
         <v>26.8</v>
       </c>
       <c r="U626" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V626" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V626" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="627" spans="1:22" x14ac:dyDescent="0.2">
@@ -43364,10 +43364,10 @@
         <v>26.8</v>
       </c>
       <c r="U627" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V627" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="V627" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="628" spans="1:22" x14ac:dyDescent="0.2">
@@ -43378,7 +43378,7 @@
         <v>106</v>
       </c>
       <c r="C628" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D628" s="14">
         <v>21</v>
@@ -43390,16 +43390,16 @@
         <v>110</v>
       </c>
       <c r="G628" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H628" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="H628" s="14" t="s">
+      <c r="I628" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="I628" s="14" t="s">
+      <c r="J628" s="14" t="s">
         <v>172</v>
-      </c>
-      <c r="J628" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="K628" s="14" t="s">
         <v>24</v>
@@ -43408,10 +43408,10 @@
         <v>58</v>
       </c>
       <c r="M628" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="N628" s="14" t="s">
         <v>174</v>
-      </c>
-      <c r="N628" s="14" t="s">
-        <v>175</v>
       </c>
       <c r="O628" s="14">
         <v>3.8</v>
@@ -43432,10 +43432,10 @@
         <v>27.05</v>
       </c>
       <c r="U628" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V628" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="629" spans="1:22" x14ac:dyDescent="0.2">
@@ -43446,7 +43446,7 @@
         <v>106</v>
       </c>
       <c r="C629" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D629" s="14">
         <v>21</v>
@@ -43458,16 +43458,16 @@
         <v>110</v>
       </c>
       <c r="G629" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H629" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="H629" s="14" t="s">
+      <c r="I629" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="I629" s="14" t="s">
+      <c r="J629" s="14" t="s">
         <v>172</v>
-      </c>
-      <c r="J629" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="K629" s="14" t="s">
         <v>24</v>
@@ -43476,10 +43476,10 @@
         <v>58</v>
       </c>
       <c r="M629" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="N629" s="14" t="s">
         <v>174</v>
-      </c>
-      <c r="N629" s="14" t="s">
-        <v>175</v>
       </c>
       <c r="O629" s="14">
         <v>3.8</v>
@@ -43500,10 +43500,10 @@
         <v>27.05</v>
       </c>
       <c r="U629" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V629" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="630" spans="1:22" x14ac:dyDescent="0.2">
@@ -43514,7 +43514,7 @@
         <v>106</v>
       </c>
       <c r="C630" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D630" s="14">
         <v>21</v>
@@ -43526,16 +43526,16 @@
         <v>110</v>
       </c>
       <c r="G630" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H630" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="H630" s="14" t="s">
+      <c r="I630" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="I630" s="14" t="s">
+      <c r="J630" s="14" t="s">
         <v>172</v>
-      </c>
-      <c r="J630" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="K630" s="14" t="s">
         <v>24</v>
@@ -43544,10 +43544,10 @@
         <v>58</v>
       </c>
       <c r="M630" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="N630" s="14" t="s">
         <v>174</v>
-      </c>
-      <c r="N630" s="14" t="s">
-        <v>175</v>
       </c>
       <c r="O630" s="14">
         <v>3.8</v>
@@ -43568,10 +43568,10 @@
         <v>27.05</v>
       </c>
       <c r="U630" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V630" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="631" spans="1:22" x14ac:dyDescent="0.2">
@@ -43582,7 +43582,7 @@
         <v>106</v>
       </c>
       <c r="C631" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D631" s="14">
         <v>21</v>
@@ -43594,16 +43594,16 @@
         <v>110</v>
       </c>
       <c r="G631" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H631" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="H631" s="14" t="s">
+      <c r="I631" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="I631" s="14" t="s">
+      <c r="J631" s="14" t="s">
         <v>172</v>
-      </c>
-      <c r="J631" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="K631" s="14" t="s">
         <v>24</v>
@@ -43612,10 +43612,10 @@
         <v>58</v>
       </c>
       <c r="M631" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="N631" s="14" t="s">
         <v>174</v>
-      </c>
-      <c r="N631" s="14" t="s">
-        <v>175</v>
       </c>
       <c r="O631" s="14">
         <v>3.8</v>
@@ -43636,10 +43636,10 @@
         <v>27.05</v>
       </c>
       <c r="U631" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V631" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="632" spans="1:22" x14ac:dyDescent="0.2">
@@ -43650,7 +43650,7 @@
         <v>106</v>
       </c>
       <c r="C632" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D632" s="14">
         <v>21</v>
@@ -43662,16 +43662,16 @@
         <v>110</v>
       </c>
       <c r="G632" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H632" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="H632" s="14" t="s">
+      <c r="I632" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="I632" s="14" t="s">
+      <c r="J632" s="14" t="s">
         <v>172</v>
-      </c>
-      <c r="J632" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="K632" s="14" t="s">
         <v>24</v>
@@ -43680,10 +43680,10 @@
         <v>58</v>
       </c>
       <c r="M632" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="N632" s="14" t="s">
         <v>174</v>
-      </c>
-      <c r="N632" s="14" t="s">
-        <v>175</v>
       </c>
       <c r="O632" s="14">
         <v>3.8</v>
@@ -43704,10 +43704,10 @@
         <v>27.05</v>
       </c>
       <c r="U632" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V632" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="633" spans="1:22" x14ac:dyDescent="0.2">
@@ -43718,7 +43718,7 @@
         <v>106</v>
       </c>
       <c r="C633" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D633" s="14">
         <v>21</v>
@@ -43730,16 +43730,16 @@
         <v>117</v>
       </c>
       <c r="G633" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H633" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="H633" s="14" t="s">
+      <c r="I633" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="I633" s="14" t="s">
+      <c r="J633" s="14" t="s">
         <v>172</v>
-      </c>
-      <c r="J633" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="K633" s="14" t="s">
         <v>24</v>
@@ -43748,10 +43748,10 @@
         <v>58</v>
       </c>
       <c r="M633" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="N633" s="14" t="s">
         <v>174</v>
-      </c>
-      <c r="N633" s="14" t="s">
-        <v>175</v>
       </c>
       <c r="O633" s="14">
         <v>3.8</v>
@@ -43772,10 +43772,10 @@
         <v>27.05</v>
       </c>
       <c r="U633" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V633" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="634" spans="1:22" x14ac:dyDescent="0.2">
@@ -43786,7 +43786,7 @@
         <v>106</v>
       </c>
       <c r="C634" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D634" s="14">
         <v>142</v>
@@ -43798,16 +43798,16 @@
         <v>110</v>
       </c>
       <c r="G634" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H634" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="H634" s="14" t="s">
+      <c r="I634" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="I634" s="14" t="s">
+      <c r="J634" s="14" t="s">
         <v>172</v>
-      </c>
-      <c r="J634" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="K634" s="14" t="s">
         <v>24</v>
@@ -43816,10 +43816,10 @@
         <v>58</v>
       </c>
       <c r="M634" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="N634" s="14" t="s">
         <v>174</v>
-      </c>
-      <c r="N634" s="14" t="s">
-        <v>175</v>
       </c>
       <c r="O634" s="14">
         <v>3.8</v>
@@ -43840,10 +43840,10 @@
         <v>27.05</v>
       </c>
       <c r="U634" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V634" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="635" spans="1:22" x14ac:dyDescent="0.2">
@@ -43854,7 +43854,7 @@
         <v>106</v>
       </c>
       <c r="C635" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D635" s="14">
         <v>142</v>
@@ -43866,16 +43866,16 @@
         <v>110</v>
       </c>
       <c r="G635" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H635" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="H635" s="14" t="s">
+      <c r="I635" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="I635" s="14" t="s">
+      <c r="J635" s="14" t="s">
         <v>172</v>
-      </c>
-      <c r="J635" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="K635" s="14" t="s">
         <v>24</v>
@@ -43884,10 +43884,10 @@
         <v>58</v>
       </c>
       <c r="M635" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="N635" s="14" t="s">
         <v>174</v>
-      </c>
-      <c r="N635" s="14" t="s">
-        <v>175</v>
       </c>
       <c r="O635" s="14">
         <v>3.8</v>
@@ -43908,10 +43908,10 @@
         <v>27.05</v>
       </c>
       <c r="U635" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V635" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="636" spans="1:22" x14ac:dyDescent="0.2">
@@ -43922,7 +43922,7 @@
         <v>106</v>
       </c>
       <c r="C636" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D636" s="14">
         <v>142</v>
@@ -43934,16 +43934,16 @@
         <v>110</v>
       </c>
       <c r="G636" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H636" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="H636" s="14" t="s">
+      <c r="I636" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="I636" s="14" t="s">
+      <c r="J636" s="14" t="s">
         <v>172</v>
-      </c>
-      <c r="J636" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="K636" s="14" t="s">
         <v>24</v>
@@ -43952,10 +43952,10 @@
         <v>58</v>
       </c>
       <c r="M636" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="N636" s="14" t="s">
         <v>174</v>
-      </c>
-      <c r="N636" s="14" t="s">
-        <v>175</v>
       </c>
       <c r="O636" s="14">
         <v>3.8</v>
@@ -43976,10 +43976,10 @@
         <v>27.05</v>
       </c>
       <c r="U636" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V636" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="637" spans="1:22" x14ac:dyDescent="0.2">
@@ -43990,7 +43990,7 @@
         <v>106</v>
       </c>
       <c r="C637" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D637" s="14">
         <v>142</v>
@@ -44002,16 +44002,16 @@
         <v>110</v>
       </c>
       <c r="G637" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H637" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="H637" s="14" t="s">
+      <c r="I637" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="I637" s="14" t="s">
+      <c r="J637" s="14" t="s">
         <v>172</v>
-      </c>
-      <c r="J637" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="K637" s="14" t="s">
         <v>24</v>
@@ -44020,10 +44020,10 @@
         <v>58</v>
       </c>
       <c r="M637" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="N637" s="14" t="s">
         <v>174</v>
-      </c>
-      <c r="N637" s="14" t="s">
-        <v>175</v>
       </c>
       <c r="O637" s="14">
         <v>3.8</v>
@@ -44044,10 +44044,10 @@
         <v>27.05</v>
       </c>
       <c r="U637" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V637" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="638" spans="1:22" x14ac:dyDescent="0.2">
@@ -44058,7 +44058,7 @@
         <v>106</v>
       </c>
       <c r="C638" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D638" s="14">
         <v>142</v>
@@ -44070,16 +44070,16 @@
         <v>117</v>
       </c>
       <c r="G638" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H638" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="H638" s="14" t="s">
+      <c r="I638" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="I638" s="14" t="s">
+      <c r="J638" s="14" t="s">
         <v>172</v>
-      </c>
-      <c r="J638" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="K638" s="14" t="s">
         <v>24</v>
@@ -44088,10 +44088,10 @@
         <v>58</v>
       </c>
       <c r="M638" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="N638" s="14" t="s">
         <v>174</v>
-      </c>
-      <c r="N638" s="14" t="s">
-        <v>175</v>
       </c>
       <c r="O638" s="14">
         <v>3.8</v>
@@ -44112,10 +44112,10 @@
         <v>27.05</v>
       </c>
       <c r="U638" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V638" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="639" spans="1:22" x14ac:dyDescent="0.2">
@@ -44126,7 +44126,7 @@
         <v>106</v>
       </c>
       <c r="C639" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D639" s="14">
         <v>142</v>
@@ -44138,16 +44138,16 @@
         <v>117</v>
       </c>
       <c r="G639" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H639" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="H639" s="14" t="s">
+      <c r="I639" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="I639" s="14" t="s">
+      <c r="J639" s="14" t="s">
         <v>172</v>
-      </c>
-      <c r="J639" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="K639" s="14" t="s">
         <v>24</v>
@@ -44156,10 +44156,10 @@
         <v>58</v>
       </c>
       <c r="M639" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="N639" s="14" t="s">
         <v>174</v>
-      </c>
-      <c r="N639" s="14" t="s">
-        <v>175</v>
       </c>
       <c r="O639" s="14">
         <v>3.8</v>
@@ -44180,10 +44180,10 @@
         <v>27.05</v>
       </c>
       <c r="U639" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V639" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerunning data cleaning scripts
</commit_message>
<xml_diff>
--- a/data/consumption_data.xlsx
+++ b/data/consumption_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6013D708-A4FD-5E45-8C93-8620556B3855}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16629CE9-C6DA-DE4B-9385-B8D1489A62F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7640" yWindow="2400" windowWidth="27560" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10840" yWindow="3020" windowWidth="27560" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10492" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10492" uniqueCount="199">
   <si>
     <t>original_unit</t>
   </si>
@@ -623,6 +623,9 @@
   <si>
     <t>above_peak_temp</t>
   </si>
+  <si>
+    <t>Zhang-etal-2017-JournalofAppliedIchtyology</t>
+  </si>
 </sst>
 </file>
 
@@ -630,8 +633,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="173" formatCode="0.000"/>
-    <numFmt numFmtId="174" formatCode="0_ "/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0_ "/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -755,19 +758,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -776,7 +779,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1122,9 +1125,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y747"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A656" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G678" sqref="G678"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35826,7 +35829,7 @@
       </c>
       <c r="U514" s="11"/>
       <c r="V514" s="4" t="s">
-        <v>158</v>
+        <v>198</v>
       </c>
     </row>
     <row r="515" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>